<commit_message>
EDA complete. Single cell solution.
</commit_message>
<xml_diff>
--- a/CH-139 Custom Grouping.xlsx
+++ b/CH-139 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0D7819-7DE1-4C38-9774-A20E0C91211B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134C288D-138B-4AC9-9B30-2713798A4377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -310,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -381,6 +381,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1395,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DCDAB9-A4C2-4C08-A79C-61A852AA71B3}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,42 +1408,58 @@
     <col min="1" max="1" width="3.109375" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.21875" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="29"/>
-      <c r="E1"/>
-      <c r="G1" s="30" t="s">
+      <c r="E1">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="K1" s="7" t="s">
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="31"/>
+      <c r="L1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2"/>
-      <c r="G2" s="6" t="s">
+      <c r="C2" s="8">
+        <v>47</v>
+      </c>
+      <c r="D2" s="32">
+        <f>(C3-C2)/C2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <f>1+D2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="33">
+        <f>IF(E2&lt;1,1,F1*E2)</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="14">
         <v>45292</v>
       </c>
@@ -1452,24 +1470,28 @@
         <f>(C4-C3)/C3</f>
         <v>0.31914893617021278</v>
       </c>
-      <c r="E3" cm="1">
-        <f t="array" ref="E3:E34">_xlfn.REDUCE(1,D3:D25,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v&gt;0,_xlfn.VSTACK(_xlpm.a,_xlpm.a*(1+_xlpm.v)),1)))</f>
-        <v>1</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="33">
+        <f t="shared" ref="E3:E26" si="0">1+D3</f>
+        <v>1.3191489361702127</v>
+      </c>
+      <c r="F3" s="33">
+        <f t="shared" ref="F3:F26" si="1">IF(E3&lt;1,1,F2*E3)</f>
+        <v>1.3191489361702127</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="27">
+      <c r="I3" s="27">
         <v>1.558139534883721</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="11"/>
+      <c r="J3" s="13"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="11"/>
+      <c r="N3" s="9"/>
+    </row>
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>45293</v>
       </c>
@@ -1477,26 +1499,31 @@
         <v>62</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D25" si="0">(C5-C4)/C4</f>
+        <f t="shared" ref="D4:D25" si="2">(C5-C4)/C4</f>
         <v>0.59677419354838712</v>
       </c>
-      <c r="E4">
-        <v>1.4423076923076923</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="33">
+        <f t="shared" si="0"/>
+        <v>1.596774193548387</v>
+      </c>
+      <c r="F4" s="33">
+        <f t="shared" si="1"/>
+        <v>2.1063829787234041</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="27">
+      <c r="I4" s="27">
         <v>-0.56565656565656564</v>
       </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="11"/>
+      <c r="J4" s="13"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="11"/>
+      <c r="N4" s="9"/>
+    </row>
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>45294</v>
       </c>
@@ -1504,22 +1531,27 @@
         <v>99</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.56565656565656564</v>
       </c>
-      <c r="E5">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="F5"/>
+      <c r="E5" s="33">
+        <f t="shared" si="0"/>
+        <v>0.43434343434343436</v>
+      </c>
+      <c r="F5" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="11"/>
+      <c r="I5"/>
+      <c r="J5" s="13"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="11"/>
+      <c r="N5" s="9"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23">
         <v>45295</v>
       </c>
@@ -1527,22 +1559,27 @@
         <v>43</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.20930232558139536</v>
       </c>
-      <c r="E6">
-        <v>1.6153846153846154</v>
-      </c>
-      <c r="F6"/>
+      <c r="E6" s="33">
+        <f t="shared" si="0"/>
+        <v>1.2093023255813953</v>
+      </c>
+      <c r="F6" s="33">
+        <f t="shared" si="1"/>
+        <v>1.2093023255813953</v>
+      </c>
       <c r="G6"/>
       <c r="H6"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="11"/>
+      <c r="I6"/>
+      <c r="J6" s="13"/>
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="11"/>
+      <c r="N6" s="9"/>
+    </row>
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23">
         <v>45296</v>
       </c>
@@ -1550,18 +1587,34 @@
         <v>52</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="E7">
-        <v>1.1190476190476191</v>
-      </c>
-      <c r="F7"/>
+      <c r="E7" s="33">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="F7" s="33">
+        <f t="shared" si="1"/>
+        <v>1.5116279069767442</v>
+      </c>
       <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="6" t="str" cm="1">
+        <f t="array" ref="H7:I9">_xlfn.LET(_xlpm.d,_xlfn.VSTACK(C3,C3:C26),
+_xlpm.dm,_xlfn.DROP(_xlpm.d,1),
+_xlpm.q,_xlfn.DROP(1+(_xlpm.dm-_xlpm.d)/_xlpm.d,-1),
+_xlpm.z, MAX(_xlfn.SCAN(1,_xlpm.q,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v&gt;1,_xlfn.IFNA(_xlpm.a*_xlpm.v,1),1))))-1,
+_xlpm.zz, MIN(_xlfn.SCAN(1,_xlpm.q,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,IF(_xlpm.v&lt;1,_xlfn.IFNA(_xlpm.a*_xlpm.v,1),1))))-1,
+_xlfn.VSTACK({"Group","Percent"},_xlfn.HSTACK(_xlfn.VSTACK("Increase","Decrease"),_xlfn.VSTACK(_xlpm.z,_xlpm.zz)))
+)</f>
+        <v>Group</v>
+      </c>
+      <c r="I7" s="20" t="str">
+        <v>Percent</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="23">
         <v>45297</v>
       </c>
@@ -1569,22 +1622,31 @@
         <v>65</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1076923076923077</v>
       </c>
-      <c r="E8">
-        <v>1.6140109890109891</v>
-      </c>
-      <c r="F8"/>
+      <c r="E8" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1076923076923078</v>
+      </c>
+      <c r="F8" s="33">
+        <f t="shared" si="1"/>
+        <v>1.6744186046511629</v>
+      </c>
       <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
+      <c r="H8" s="12" t="str">
+        <v>Increase</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1.558139534883721</v>
+      </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
-    </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N8"/>
+    </row>
+    <row r="9" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23">
         <v>45298</v>
       </c>
@@ -1592,22 +1654,31 @@
         <v>72</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.52777777777777779</v>
       </c>
-      <c r="E9">
-        <v>1.2533333333333334</v>
-      </c>
-      <c r="F9"/>
-      <c r="G9" s="5"/>
-      <c r="H9"/>
-      <c r="I9"/>
+      <c r="E9" s="33">
+        <f t="shared" si="0"/>
+        <v>1.5277777777777777</v>
+      </c>
+      <c r="F9" s="33">
+        <f t="shared" si="1"/>
+        <v>2.558139534883721</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" s="12" t="str">
+        <v>Decrease</v>
+      </c>
+      <c r="I9" s="27">
+        <v>-0.56565656565656564</v>
+      </c>
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
       <c r="M9"/>
-    </row>
-    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23">
         <v>45299</v>
       </c>
@@ -1615,22 +1686,27 @@
         <v>110</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-3.6363636363636362E-2</v>
       </c>
-      <c r="E10">
-        <v>1.8076923076923077</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" s="5"/>
-      <c r="H10"/>
+      <c r="E10" s="33">
+        <f t="shared" si="0"/>
+        <v>0.96363636363636362</v>
+      </c>
+      <c r="F10" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" s="5"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
-    </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N10"/>
+    </row>
+    <row r="11" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="16">
         <v>45300</v>
       </c>
@@ -1638,22 +1714,27 @@
         <v>106</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-9.433962264150943E-3</v>
       </c>
-      <c r="E11">
-        <v>1.0851063829787233</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" s="5"/>
-      <c r="H11"/>
+      <c r="E11" s="33">
+        <f t="shared" si="0"/>
+        <v>0.99056603773584906</v>
+      </c>
+      <c r="F11" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" s="5"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
-    </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="16">
         <v>45301</v>
       </c>
@@ -1661,23 +1742,28 @@
         <v>105</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.9047619047619049E-2</v>
       </c>
-      <c r="E12">
-        <v>1.5650572831423895</v>
-      </c>
-      <c r="F12"/>
-      <c r="G12" s="5"/>
-      <c r="H12"/>
+      <c r="E12" s="33">
+        <f t="shared" si="0"/>
+        <v>0.98095238095238091</v>
+      </c>
+      <c r="F12" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12" s="5"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12"/>
       <c r="N12"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O12"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="16">
         <v>45302</v>
       </c>
@@ -1685,14 +1771,19 @@
         <v>103</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-2.9126213592233011E-2</v>
       </c>
-      <c r="E13">
-        <v>1.2153191489361703</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E13" s="33">
+        <f t="shared" si="0"/>
+        <v>0.970873786407767</v>
+      </c>
+      <c r="F13" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="16">
         <v>45303</v>
       </c>
@@ -1700,14 +1791,19 @@
         <v>100</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.15</v>
       </c>
-      <c r="E14">
-        <v>1.7528641571194761</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E14" s="33">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F14" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="16">
         <v>45304</v>
@@ -1716,14 +1812,19 @@
         <v>85</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f>(C16-C15)/C15</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="E15">
-        <v>1.2142857142857142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E15" s="33">
+        <f t="shared" si="0"/>
+        <v>1.0588235294117647</v>
+      </c>
+      <c r="F15" s="33">
+        <f t="shared" si="1"/>
+        <v>1.0588235294117647</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="25">
         <v>45305</v>
@@ -1732,14 +1833,19 @@
         <v>90</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.1111111111111111</v>
       </c>
-      <c r="E16">
-        <v>1.7513736263736261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E16" s="33">
+        <f t="shared" si="0"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F16" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="25">
         <v>45306</v>
@@ -1748,14 +1854,19 @@
         <v>80</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-0.23749999999999999</v>
       </c>
-      <c r="E17">
-        <v>1.3599999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E17" s="33">
+        <f t="shared" si="0"/>
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="F17" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="25">
         <v>45307</v>
@@ -1764,14 +1875,19 @@
         <v>61</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-1.6393442622950821E-2</v>
       </c>
-      <c r="E18">
-        <v>1.9615384615384615</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E18" s="33">
+        <f t="shared" si="0"/>
+        <v>0.98360655737704916</v>
+      </c>
+      <c r="F18" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="25">
         <v>45308</v>
@@ -1780,14 +1896,19 @@
         <v>60</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-8.3333333333333329E-2</v>
       </c>
-      <c r="E19">
-        <v>1.0294117647058822</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E19" s="33">
+        <f t="shared" si="0"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="F19" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="25">
         <v>45309</v>
@@ -1796,14 +1917,19 @@
         <v>55</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-5.4545454545454543E-2</v>
       </c>
-      <c r="E20">
-        <v>1.4847285067873301</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E20" s="33">
+        <f t="shared" si="0"/>
+        <v>0.94545454545454544</v>
+      </c>
+      <c r="F20" s="33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="25">
         <v>45310</v>
@@ -1812,14 +1938,19 @@
         <v>52</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.44230769230769229</v>
       </c>
-      <c r="E21">
-        <v>1.1529411764705881</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E21" s="33">
+        <f t="shared" si="0"/>
+        <v>1.4423076923076923</v>
+      </c>
+      <c r="F21" s="33">
+        <f t="shared" si="1"/>
+        <v>1.4423076923076923</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="18">
         <v>45311</v>
@@ -1828,15 +1959,20 @@
         <v>75</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="E22">
-        <v>1.6628959276018098</v>
-      </c>
-      <c r="N22" s="2"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E22" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F22" s="33">
+        <f t="shared" si="1"/>
+        <v>1.6153846153846154</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="18">
         <v>45312</v>
@@ -1845,14 +1981,19 @@
         <v>84</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11904761904761904</v>
       </c>
-      <c r="E23">
-        <v>1.1519607843137254</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E23" s="33">
+        <f t="shared" si="0"/>
+        <v>1.1190476190476191</v>
+      </c>
+      <c r="F23" s="33">
+        <f t="shared" si="1"/>
+        <v>1.8076923076923077</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B24" s="18">
         <v>45313</v>
       </c>
@@ -1860,14 +2001,19 @@
         <v>94</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="E24">
-        <v>1.6614819004524886</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E24" s="33">
+        <f t="shared" si="0"/>
+        <v>1.0851063829787233</v>
+      </c>
+      <c r="F24" s="33">
+        <f t="shared" si="1"/>
+        <v>1.9615384615384615</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B25" s="18">
         <v>45314</v>
       </c>
@@ -1875,68 +2021,38 @@
         <v>102</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="E25">
-        <v>1.2901960784313724</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E25" s="33">
+        <f t="shared" si="0"/>
+        <v>1.0294117647058822</v>
+      </c>
+      <c r="F25" s="33">
+        <f t="shared" si="1"/>
+        <v>2.0192307692307687</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B26" s="21">
         <v>45315</v>
       </c>
       <c r="C26" s="22">
         <v>105</v>
       </c>
-      <c r="E26">
-        <v>1.8608597285067872</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E27">
-        <v>1.1170212765957446</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E28">
-        <v>1.6110883797054008</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E29">
-        <v>1.2510638297872341</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E30">
-        <v>1.8044189852700487</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E31">
-        <v>1.2499999999999998</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="E32">
-        <v>1.802884615384615</v>
-      </c>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33">
-        <v>1.3999999999999997</v>
-      </c>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34">
+      <c r="E26" s="33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F26" s="33">
+        <f t="shared" si="1"/>
         <v>2.0192307692307687</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on understanding Alt1
</commit_message>
<xml_diff>
--- a/CH-139 Custom Grouping.xlsx
+++ b/CH-139 Custom Grouping.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445BEA56-5525-4D23-A9F6-21842312CF8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FA0965-691F-4094-8CE3-FF2D15FA7DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -96,7 +98,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +124,14 @@
       <color theme="1"/>
       <name val="Corbel"/>
       <family val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Corbel"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -307,10 +317,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -369,6 +380,8 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -381,10 +394,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,12 +1021,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="629" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{5D2FD712-6E10-4BD6-8A77-36FF06E2C73D}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1022,16 +1067,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="31"/>
       <c r="E1"/>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="K1" s="7" t="s">
+      <c r="H1" s="33"/>
+      <c r="K1" s="34" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1389,9 +1434,12 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{8F7DFD66-AB40-4AFB-8316-356A9E4C7D2E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1399,8 +1447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DCDAB9-A4C2-4C08-A79C-61A852AA71B3}">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView topLeftCell="A18" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,20 +1463,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="31"/>
       <c r="E1">
         <v>1</v>
       </c>
       <c r="F1">
         <v>1</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="31"/>
+      <c r="I1" s="33"/>
       <c r="L1" s="7" t="s">
         <v>8</v>
       </c>
@@ -1440,15 +1488,15 @@
       <c r="C2" s="8">
         <v>47</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="28">
         <f>(C3-C2)/C2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="33">
+      <c r="E2" s="29">
         <f>1+D2</f>
         <v>1</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="29">
         <f>IF(E2&lt;1,1,F1*E2)</f>
         <v>1</v>
       </c>
@@ -1470,11 +1518,11 @@
         <f>(C4-C3)/C3</f>
         <v>0.31914893617021278</v>
       </c>
-      <c r="E3" s="33">
+      <c r="E3" s="29">
         <f t="shared" ref="E3:E26" si="0">1+D3</f>
         <v>1.3191489361702127</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="29">
         <f t="shared" ref="F3:F26" si="1">IF(E3&lt;1,1,F2*E3)</f>
         <v>1.3191489361702127</v>
       </c>
@@ -1502,11 +1550,11 @@
         <f t="shared" ref="D4:D25" si="2">(C5-C4)/C4</f>
         <v>0.59677419354838712</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="29">
         <f t="shared" si="0"/>
         <v>1.596774193548387</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="29">
         <f t="shared" si="1"/>
         <v>2.1063829787234041</v>
       </c>
@@ -1534,11 +1582,11 @@
         <f t="shared" si="2"/>
         <v>-0.56565656565656564</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="29">
         <f t="shared" si="0"/>
         <v>0.43434343434343436</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1562,11 +1610,11 @@
         <f t="shared" si="2"/>
         <v>0.20930232558139536</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="29">
         <f t="shared" si="0"/>
         <v>1.2093023255813953</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="29">
         <f t="shared" si="1"/>
         <v>1.2093023255813953</v>
       </c>
@@ -1590,11 +1638,11 @@
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="29">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="29">
         <f t="shared" si="1"/>
         <v>1.5116279069767442</v>
       </c>
@@ -1625,11 +1673,11 @@
         <f t="shared" si="2"/>
         <v>0.1076923076923077</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="29">
         <f t="shared" si="0"/>
         <v>1.1076923076923078</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="29">
         <f t="shared" si="1"/>
         <v>1.6744186046511629</v>
       </c>
@@ -1657,11 +1705,11 @@
         <f t="shared" si="2"/>
         <v>0.52777777777777779</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="29">
         <f t="shared" si="0"/>
         <v>1.5277777777777777</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="29">
         <f t="shared" si="1"/>
         <v>2.558139534883721</v>
       </c>
@@ -1689,11 +1737,11 @@
         <f t="shared" si="2"/>
         <v>-3.6363636363636362E-2</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="29">
         <f t="shared" si="0"/>
         <v>0.96363636363636362</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1717,11 +1765,11 @@
         <f t="shared" si="2"/>
         <v>-9.433962264150943E-3</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="29">
         <f t="shared" si="0"/>
         <v>0.99056603773584906</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1755,11 +1803,11 @@
         <f t="shared" si="2"/>
         <v>-1.9047619047619049E-2</v>
       </c>
-      <c r="E12" s="33">
+      <c r="E12" s="29">
         <f t="shared" si="0"/>
         <v>0.98095238095238091</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1788,11 +1836,11 @@
         <f t="shared" si="2"/>
         <v>-2.9126213592233011E-2</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="29">
         <f t="shared" si="0"/>
         <v>0.970873786407767</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1814,11 +1862,11 @@
         <f t="shared" si="2"/>
         <v>-0.15</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="29">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1835,11 +1883,11 @@
         <f>(C16-C15)/C15</f>
         <v>5.8823529411764705E-2</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="29">
         <f t="shared" si="0"/>
         <v>1.0588235294117647</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="29">
         <f t="shared" si="1"/>
         <v>1.0588235294117647</v>
       </c>
@@ -1856,11 +1904,11 @@
         <f t="shared" si="2"/>
         <v>-0.1111111111111111</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="29">
         <f t="shared" si="0"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1877,11 +1925,11 @@
         <f t="shared" si="2"/>
         <v>-0.23749999999999999</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="29">
         <f t="shared" si="0"/>
         <v>0.76249999999999996</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1898,11 +1946,11 @@
         <f t="shared" si="2"/>
         <v>-1.6393442622950821E-2</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="29">
         <f t="shared" si="0"/>
         <v>0.98360655737704916</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1919,11 +1967,11 @@
         <f t="shared" si="2"/>
         <v>-8.3333333333333329E-2</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="29">
         <f t="shared" si="0"/>
         <v>0.91666666666666663</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1940,11 +1988,11 @@
         <f t="shared" si="2"/>
         <v>-5.4545454545454543E-2</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="29">
         <f t="shared" si="0"/>
         <v>0.94545454545454544</v>
       </c>
-      <c r="F20" s="33">
+      <c r="F20" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1961,11 +2009,11 @@
         <f t="shared" si="2"/>
         <v>0.44230769230769229</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="29">
         <f t="shared" si="0"/>
         <v>1.4423076923076923</v>
       </c>
-      <c r="F21" s="33">
+      <c r="F21" s="29">
         <f t="shared" si="1"/>
         <v>1.4423076923076923</v>
       </c>
@@ -1982,11 +2030,11 @@
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="29">
         <f t="shared" si="0"/>
         <v>1.1200000000000001</v>
       </c>
-      <c r="F22" s="33">
+      <c r="F22" s="29">
         <f t="shared" si="1"/>
         <v>1.6153846153846154</v>
       </c>
@@ -2004,11 +2052,11 @@
         <f t="shared" si="2"/>
         <v>0.11904761904761904</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="29">
         <f t="shared" si="0"/>
         <v>1.1190476190476191</v>
       </c>
-      <c r="F23" s="33">
+      <c r="F23" s="29">
         <f t="shared" si="1"/>
         <v>1.8076923076923077</v>
       </c>
@@ -2024,11 +2072,11 @@
         <f t="shared" si="2"/>
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="E24" s="33">
+      <c r="E24" s="29">
         <f t="shared" si="0"/>
         <v>1.0851063829787233</v>
       </c>
-      <c r="F24" s="33">
+      <c r="F24" s="29">
         <f t="shared" si="1"/>
         <v>1.9615384615384615</v>
       </c>
@@ -2044,11 +2092,11 @@
         <f t="shared" si="2"/>
         <v>2.9411764705882353E-2</v>
       </c>
-      <c r="E25" s="33">
+      <c r="E25" s="29">
         <f t="shared" si="0"/>
         <v>1.0294117647058822</v>
       </c>
-      <c r="F25" s="33">
+      <c r="F25" s="29">
         <f t="shared" si="1"/>
         <v>2.0192307692307687</v>
       </c>
@@ -2060,11 +2108,11 @@
       <c r="C26" s="22">
         <v>105</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="29">
         <f t="shared" si="1"/>
         <v>2.0192307692307687</v>
       </c>
@@ -2077,4 +2125,824 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2537058D-8066-453F-8E56-AFF03DEA6AFA}">
+  <dimension ref="A1:N63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="E1"/>
+      <c r="G1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="33"/>
+      <c r="K1" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="15">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3"/>
+      <c r="G3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="27">
+        <v>1.558139534883721</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="15">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4"/>
+      <c r="G4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="27">
+        <v>-0.56565656565656564</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="15">
+        <v>99</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="23">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="24">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="24">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="24">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="24">
+        <v>72</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6" t="str" cm="1">
+        <f t="array" ref="E9:F11">_xlfn.LET(
+    _xlpm.s, C3:C26,
+    _xlfn.VSTACK(
+        {"Group","Percent"},
+        _xlfn.HSTACK(
+            {"Increase";"Decrease"},
+            _xlfn.TAKE(
+                _xlfn._xlws.SORT(
+                    _xlpm.s /
+                        _xlfn.SCAN(
+                            ,
+                            _xlpm.s,
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                                _xlfn.LET(
+                                    _xlpm.b, _xlfn.TAKE(INDEX(_xlpm.s, 1):_xlpm.v, -3),
+                                    IF(_xlfn.XOR(_xlfn.DROP(_xlpm.b, 1) &gt; _xlfn.DROP(_xlpm.b, -1)), _xlfn.SINGLE(+_xlfn.TAKE(_xlpm.b, -2)), _xlpm.a)
+                                )
+                            )
+                        ) - 1
+                ),
+                {-1;1}
+            )
+        )
+    )
+)</f>
+        <v>Group</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <v>Percent</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="23">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="24">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="12" t="str">
+        <v>Increase</v>
+      </c>
+      <c r="F10" s="27">
+        <v>1.558139534883721</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="17">
+        <v>106</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="12" t="str">
+        <v>Decrease</v>
+      </c>
+      <c r="F11" s="27">
+        <v>-0.56565656565656564</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="17">
+        <v>105</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+      <c r="G12" s="5"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="17">
+        <v>103</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="17">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="17">
+        <v>85</v>
+      </c>
+      <c r="E15" s="35" cm="1">
+        <f t="array" ref="E15:E38">_xlfn.SCAN(
+                            ,
+                            C3:C26,
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                                _xlfn.LET(
+                                    _xlpm.b, _xlfn.TAKE(INDEX(C3:C26, 1):_xlpm.v, -3),
+                                    IF(_xlfn.XOR(_xlfn.DROP(_xlpm.b, 1) &gt; _xlfn.DROP(_xlpm.b, -1)), _xlfn.SINGLE(+_xlfn.TAKE(_xlpm.b, -2)), _xlpm.a)
+                                )
+                            )
+                        )</f>
+        <v>47</v>
+      </c>
+      <c r="F15" cm="1">
+        <f t="array" ref="F15:F38" xml:space="preserve"> C3:C26/_xlfn.ANCHORARRAY(E15)</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="5">
+        <f>F15-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="25">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="26">
+        <v>90</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="35">
+        <v>47</v>
+      </c>
+      <c r="F16">
+        <v>1.3191489361702127</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" ref="G16:G38" si="0">F16-1</f>
+        <v>0.31914893617021267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="25">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="26">
+        <v>80</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="35">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <v>2.1063829787234041</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1063829787234041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="25">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="26">
+        <v>61</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="35">
+        <v>99</v>
+      </c>
+      <c r="F18">
+        <v>0.43434343434343436</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.56565656565656564</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="25">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="26">
+        <v>60</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="35">
+        <v>43</v>
+      </c>
+      <c r="F19">
+        <v>1.2093023255813953</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.20930232558139528</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="25">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="26">
+        <v>55</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="35">
+        <v>43</v>
+      </c>
+      <c r="F20">
+        <v>1.5116279069767442</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.51162790697674421</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="25">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="26">
+        <v>52</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="35">
+        <v>43</v>
+      </c>
+      <c r="F21">
+        <v>1.6744186046511629</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.67441860465116288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="18">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="19">
+        <v>75</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="35">
+        <v>43</v>
+      </c>
+      <c r="F22">
+        <v>2.558139534883721</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>1.558139534883721</v>
+      </c>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="18">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="19">
+        <v>84</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="35">
+        <v>110</v>
+      </c>
+      <c r="F23">
+        <v>0.96363636363636362</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="0"/>
+        <v>-3.6363636363636376E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="18">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="19">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="35">
+        <v>110</v>
+      </c>
+      <c r="F24">
+        <v>0.95454545454545459</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="0"/>
+        <v>-4.5454545454545414E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="18">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="19">
+        <v>102</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="35">
+        <v>110</v>
+      </c>
+      <c r="F25">
+        <v>0.9363636363636364</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>-6.3636363636363602E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="21">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="22">
+        <v>105</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="35">
+        <v>110</v>
+      </c>
+      <c r="F26">
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="0"/>
+        <v>-9.0909090909090939E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E27" s="35">
+        <v>110</v>
+      </c>
+      <c r="F27">
+        <v>0.77272727272727271</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.22727272727272729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E28" s="35">
+        <v>85</v>
+      </c>
+      <c r="F28">
+        <v>1.0588235294117647</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8823529411764719E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E29" s="35">
+        <v>90</v>
+      </c>
+      <c r="F29">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.11111111111111116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E30" s="35">
+        <v>90</v>
+      </c>
+      <c r="F30">
+        <v>0.67777777777777781</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.32222222222222219</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E31" s="35">
+        <v>90</v>
+      </c>
+      <c r="F31">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="E32" s="35">
+        <v>90</v>
+      </c>
+      <c r="F32">
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.38888888888888884</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="35">
+        <v>90</v>
+      </c>
+      <c r="F33">
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="G33" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.42222222222222228</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="35">
+        <v>52</v>
+      </c>
+      <c r="F34">
+        <v>1.4423076923076923</v>
+      </c>
+      <c r="G34" s="5">
+        <f t="shared" si="0"/>
+        <v>0.44230769230769229</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="35">
+        <v>52</v>
+      </c>
+      <c r="F35">
+        <v>1.6153846153846154</v>
+      </c>
+      <c r="G35" s="5">
+        <f t="shared" si="0"/>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="35">
+        <v>52</v>
+      </c>
+      <c r="F36">
+        <v>1.8076923076923077</v>
+      </c>
+      <c r="G36" s="5">
+        <f t="shared" si="0"/>
+        <v>0.80769230769230771</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="35">
+        <v>52</v>
+      </c>
+      <c r="F37">
+        <v>1.9615384615384615</v>
+      </c>
+      <c r="G37" s="5">
+        <f t="shared" si="0"/>
+        <v>0.96153846153846145</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="35">
+        <v>52</v>
+      </c>
+      <c r="F38">
+        <v>2.0192307692307692</v>
+      </c>
+      <c r="G38" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0192307692307692</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" cm="1">
+        <f t="array" ref="E40:E63">_xlfn.SCAN(
+                            ,
+                            C3:C26,
+                            _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                                _xlfn.LET(
+                                    _xlpm.b, _xlfn.TAKE(INDEX(C3:C26, 1):_xlpm.v, -3),
+                                    _xlfn.TEXTJOIN(",",,_xlpm.b)
+                                )
+                            )
+                        )</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" t="str">
+        <v>47,62</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" t="str">
+        <v>47,62,99</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" t="str">
+        <v>62,99,43</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" t="str">
+        <v>99,43,52</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" t="str">
+        <v>43,52,65</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" t="str">
+        <v>52,65,72</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" t="str">
+        <v>65,72,110</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" t="str">
+        <v>72,110,106</v>
+      </c>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" t="str">
+        <v>110,106,105</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" t="str">
+        <v>106,105,103</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" t="str">
+        <v>105,103,100</v>
+      </c>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" t="str">
+        <v>103,100,85</v>
+      </c>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E53" t="str">
+        <v>100,85,90</v>
+      </c>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E54" t="str">
+        <v>85,90,80</v>
+      </c>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E55" t="str">
+        <v>90,80,61</v>
+      </c>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E56" t="str">
+        <v>80,61,60</v>
+      </c>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E57" t="str">
+        <v>61,60,55</v>
+      </c>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E58" t="str">
+        <v>60,55,52</v>
+      </c>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E59" t="str">
+        <v>55,52,75</v>
+      </c>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E60" t="str">
+        <v>52,75,84</v>
+      </c>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E61" t="str">
+        <v>75,84,94</v>
+      </c>
+    </row>
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E62" t="str">
+        <v>84,94,102</v>
+      </c>
+    </row>
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E63" t="str">
+        <v>94,102,105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{B0805BD1-C71D-41AB-8A4E-7FC8E908C30E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Alt2, still working on Alt1
</commit_message>
<xml_diff>
--- a/CH-139 Custom Grouping.xlsx
+++ b/CH-139 Custom Grouping.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FA0965-691F-4094-8CE3-FF2D15FA7DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60ADFE91-BB59-4A2C-A101-0318678966E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
+    <sheet name="Alt2" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alt1'!$B$2:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Alt2'!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$D$26</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$D$26</definedName>
   </definedNames>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>Question</t>
   </si>
@@ -2131,7 +2133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2537058D-8066-453F-8E56-AFF03DEA6AFA}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2945,4 +2947,405 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862630FE-0C64-4F68-B55D-7D50567D4860}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="E1"/>
+      <c r="G1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="33"/>
+      <c r="K1" s="34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2"/>
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14">
+        <v>45292</v>
+      </c>
+      <c r="C3" s="15">
+        <v>47</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3"/>
+      <c r="G3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="27">
+        <v>1.558139534883721</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="14">
+        <v>45293</v>
+      </c>
+      <c r="C4" s="15">
+        <v>62</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4"/>
+      <c r="G4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="27">
+        <v>-0.56565656565656564</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14">
+        <v>45294</v>
+      </c>
+      <c r="C5" s="15">
+        <v>99</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="23">
+        <v>45295</v>
+      </c>
+      <c r="C6" s="24">
+        <v>43</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23">
+        <v>45296</v>
+      </c>
+      <c r="C7" s="24">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="23">
+        <v>45297</v>
+      </c>
+      <c r="C8" s="24">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+    </row>
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="23">
+        <v>45298</v>
+      </c>
+      <c r="C9" s="24">
+        <v>72</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9"/>
+      <c r="G9" s="5"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="23">
+        <v>45299</v>
+      </c>
+      <c r="C10" s="24">
+        <v>110</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10"/>
+      <c r="G10" s="5"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="16">
+        <v>45300</v>
+      </c>
+      <c r="C11" s="17">
+        <v>106</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11"/>
+      <c r="G11" s="5"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="16">
+        <v>45301</v>
+      </c>
+      <c r="C12" s="17">
+        <v>105</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12"/>
+      <c r="G12" s="5"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" s="16">
+        <v>45302</v>
+      </c>
+      <c r="C13" s="17">
+        <v>103</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" s="16">
+        <v>45303</v>
+      </c>
+      <c r="C14" s="17">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="16">
+        <v>45304</v>
+      </c>
+      <c r="C15" s="17">
+        <v>85</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="25">
+        <v>45305</v>
+      </c>
+      <c r="C16" s="26">
+        <v>90</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10" t="str" cm="1">
+        <f t="array" ref="E16:F17">_xlfn.LET(_xlpm.a,DAY(B3:B26),_xlpm.b,C3:C26,_xlpm.c,_xlpm.b/_xlfn.IFNA(_xlfn.XLOOKUP(_xlpm.a-_xlfn.TOROW(_xlpm.a),_xlpm.a,_xlpm.b),_xlpm.b)-1,_xlfn.HSTACK({"Inc";"Dec"}&amp;"rease",_xlfn.VSTACK(MAX(_xlpm.c),MIN(_xlpm.c))))</f>
+        <v>Increase</v>
+      </c>
+      <c r="F16">
+        <v>1.558139534883721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="25">
+        <v>45306</v>
+      </c>
+      <c r="C17" s="26">
+        <v>80</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10" t="str">
+        <v>Decrease</v>
+      </c>
+      <c r="F17">
+        <v>-0.56565656565656564</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="25">
+        <v>45307</v>
+      </c>
+      <c r="C18" s="26">
+        <v>61</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="25">
+        <v>45308</v>
+      </c>
+      <c r="C19" s="26">
+        <v>60</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="25">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="26">
+        <v>55</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="25">
+        <v>45310</v>
+      </c>
+      <c r="C21" s="26">
+        <v>52</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="18">
+        <v>45311</v>
+      </c>
+      <c r="C22" s="19">
+        <v>75</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1"/>
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="18">
+        <v>45312</v>
+      </c>
+      <c r="C23" s="19">
+        <v>84</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="18">
+        <v>45313</v>
+      </c>
+      <c r="C24" s="19">
+        <v>94</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="18">
+        <v>45314</v>
+      </c>
+      <c r="C25" s="19">
+        <v>102</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="21">
+        <v>45315</v>
+      </c>
+      <c r="C26" s="22">
+        <v>105</v>
+      </c>
+      <c r="D26" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K1" r:id="rId1" xr:uid="{87AF2F03-ACB9-464C-91E9-6CB7EF123652}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Alt1 now making sense
</commit_message>
<xml_diff>
--- a/CH-139 Custom Grouping.xlsx
+++ b/CH-139 Custom Grouping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22BD925-D4A6-4516-9D52-8A05E249C9B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3024DA1A-0A8B-4167-9C4E-BC8994D212E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2143,8 +2143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2537058D-8066-453F-8E56-AFF03DEA6AFA}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2902,7 +2902,7 @@
         <v>72,110,106</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E49" t="str">
         <v>110,106,105</v>
       </c>
@@ -2911,72 +2911,111 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E50" t="str">
         <v>106,105,103</v>
       </c>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E51" t="str">
         <v>105,103,100</v>
       </c>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E52" t="str">
         <v>103,100,85</v>
       </c>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E53" t="str">
         <v>100,85,90</v>
       </c>
-    </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F53" t="str" cm="1">
+        <f t="array" ref="F53:F55">_xlfn.TEXTSPLIT(E53,,",")</f>
+        <v>100</v>
+      </c>
+      <c r="G53" s="5" t="str" cm="1">
+        <f t="array" ref="G53:G54">_xlfn.DROP(F53:F55,1)</f>
+        <v>85</v>
+      </c>
+      <c r="H53" t="str" cm="1">
+        <f t="array" ref="H53:H54">_xlfn.DROP(F53:F55,-1)</f>
+        <v>100</v>
+      </c>
+      <c r="I53" t="str" cm="1">
+        <f t="array" ref="I53">_xlfn.SINGLE(+_xlfn.TAKE(_xlfn.ANCHORARRAY(F53),-2))</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E54" t="str">
         <v>85,90,80</v>
       </c>
-    </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F54" t="str">
+        <v>85</v>
+      </c>
+      <c r="G54" s="5" t="str">
+        <v>90</v>
+      </c>
+      <c r="H54" t="str">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E55" t="str">
         <v>90,80,61</v>
       </c>
-    </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="F55" t="str">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E56" t="str">
         <v>80,61,60</v>
       </c>
-    </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G56" s="5" t="b" cm="1">
+        <f t="array" ref="G56:G57">_xlfn.ANCHORARRAY(G53)&gt;_xlfn.ANCHORARRAY(H53)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E57" t="str">
         <v>61,60,55</v>
       </c>
-    </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E58" t="str">
         <v>60,55,52</v>
       </c>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E59" t="str">
         <v>55,52,75</v>
       </c>
-    </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G59" s="36" t="b">
+        <f>_xlfn.XOR(_xlfn.ANCHORARRAY(G56))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E60" t="str">
         <v>52,75,84</v>
       </c>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E61" t="str">
         <v>75,84,94</v>
       </c>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E62" t="str">
         <v>84,94,102</v>
       </c>
     </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E63" t="str">
         <v>94,102,105</v>
       </c>

</xml_diff>